<commit_message>
data-model: Correct JSON keys for project name and alternate names
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/project.xlsx
+++ b/indigo/spreadsheetform_guides/project.xlsx
@@ -67,7 +67,7 @@
     <t xml:space="preserve">Impact Bond Name</t>
   </si>
   <si>
-    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:name</t>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:name/value</t>
   </si>
   <si>
     <t xml:space="preserve">Alternative Names</t>
@@ -76,7 +76,7 @@
     <t xml:space="preserve">(comma sep)</t>
   </si>
   <si>
-    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:alternative_names</t>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:alternative_names/value</t>
   </si>
   <si>
     <t xml:space="preserve">Stage of Development</t>
@@ -1541,7 +1541,7 @@
   <dimension ref="A2:F79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1601,7 +1601,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -2337,7 +2337,7 @@
   <dimension ref="A3:M39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
+      <selection pane="topLeft" activeCell="K11" activeCellId="1" sqref="C10:C11 K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2938,7 +2938,7 @@
   <dimension ref="A5:N38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
+      <selection pane="topLeft" activeCell="K9" activeCellId="1" sqref="C10:C11 K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3569,7 +3569,7 @@
   <dimension ref="A2:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="C10:C11 B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3804,7 +3804,7 @@
   <dimension ref="A2:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O25" activeCellId="0" sqref="O25"/>
+      <selection pane="topLeft" activeCell="O25" activeCellId="1" sqref="C10:C11 O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4038,7 +4038,7 @@
   <dimension ref="A2:I33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
+      <selection pane="topLeft" activeCell="K16" activeCellId="1" sqref="C10:C11 K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4469,7 +4469,7 @@
   <dimension ref="A2:J32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="1" sqref="C10:C11 H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4928,7 +4928,7 @@
   <dimension ref="A2:I36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="topLeft" activeCell="I8" activeCellId="1" sqref="C10:C11 I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5361,7 +5361,7 @@
   <dimension ref="A7:J37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5811,7 +5811,7 @@
   <dimension ref="A2:M37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
+      <selection pane="topLeft" activeCell="H16" activeCellId="1" sqref="C10:C11 H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6404,7 +6404,7 @@
   <dimension ref="A2:N39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L11" activeCellId="0" sqref="L11"/>
+      <selection pane="topLeft" activeCell="L11" activeCellId="1" sqref="C10:C11 L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7045,7 +7045,7 @@
   <dimension ref="A3:N46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
+      <selection pane="topLeft" activeCell="G29" activeCellId="1" sqref="C10:C11 G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7738,7 +7738,7 @@
   <dimension ref="A2:F41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="1" sqref="C10:C11 A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
data-model: Results table - "id" column should be "outcome_metric_id"
https://github.com/INDIGO-Initiative/database-app/issues/12
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/project.xlsx
+++ b/indigo/spreadsheetform_guides/project.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="General Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -1010,7 +1010,8 @@
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_metrics:status</t>
   </si>
   <si>
-    <t xml:space="preserve">Outcome Id</t>
+    <t xml:space="preserve">Outcome 
+Metric Id</t>
   </si>
   <si>
     <t xml:space="preserve">Result level</t>
@@ -1043,7 +1044,7 @@
     <t xml:space="preserve">(source ids, comma seperated)</t>
   </si>
   <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:results:id</t>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:results:outcome_metric_id</t>
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:results:result_level/value</t>
@@ -1274,7 +1275,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1340,6 +1341,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1422,7 +1427,7 @@
   </sheetPr>
   <dimension ref="A2:F67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A65" activeCellId="0" sqref="A65"/>
     </sheetView>
   </sheetViews>
@@ -2165,19 +2170,19 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C11" type="list">
-      <formula1>"Early-stage design,Late-stage design,Contracted,Implementation,Service delivery complete,Complete,"</formula1>
+      <formula1>"Early-stage design,Late-stage design,Contracted,Implementation,Service delivery complete,Complete"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C47" type="list">
-      <formula1>"Employment and training,Child and family welfare,Health,Homelessness,Education,Criminal justice,Agriculture and environment,Poverty reduction,"</formula1>
+      <formula1>"Employment and training,Child and family welfare,Health,Homelessness,Education,Criminal justice,Agriculture and environment,Poverty reduction"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C58" type="list">
-      <formula1>"Individual,Other,"</formula1>
+      <formula1>"Individual,Other"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C64" type="list">
-      <formula1>"Pause project,Continue on outcomes contract without variations,Continue on outcomes contract with variations,Switch to grant payments based on medium scenarios,"</formula1>
+      <formula1>"Pause project,Continue on outcomes contract without variations,Continue on outcomes contract with variations,Switch to grant payments based on medium scenarios"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -2755,15 +2760,15 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E4:E32" type="list">
-      <formula1>"Individual,Other,"</formula1>
+      <formula1>"Individual,Other"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I4:I32" type="list">
-      <formula1>"RCT,Quasi-experimental,Historical comparison,Pre-post analysis,Simple Ex-post verification ,Not available,"</formula1>
+      <formula1>"RCT,Quasi-experimental,Historical comparison,Pre-post analysis,Simple Ex-post verification ,Not available"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J4:J32" type="list">
-      <formula1>"Existing administrative data,New data collected,"</formula1>
+      <formula1>"Existing administrative data,New data collected"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -2784,7 +2789,7 @@
   </sheetPr>
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2827,7 +2832,7 @@
       <c r="N2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="17" t="s">
         <v>321</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -2890,7 +2895,7 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="72.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
         <v>331</v>
       </c>
@@ -3392,11 +3397,11 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5:B33" type="list">
-      <formula1>"Project level,Outcome level,"</formula1>
+      <formula1>"Project level,Outcome level"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C5:C33" type="list">
-      <formula1>"Interim,Final,"</formula1>
+      <formula1>"Interim,Final"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -5198,7 +5203,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C4:C32" type="list">
-      <formula1>"Contract,Report,Award notice,Website,"</formula1>
+      <formula1>"Contract,Report,Award notice,Website"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -6264,7 +6269,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C4:C32" type="list">
-      <formula1>"Nonprofit/NGO,Foundation/Philanthropist,Government/Public Sector/Public Bank,For-profit,Other,"</formula1>
+      <formula1>"Nonprofit/NGO,Foundation/Philanthropist,Government/Public Sector/Public Bank,For-profit,Other"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -6954,11 +6959,11 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B4:B32" type="list">
-      <formula1>"Nonprofit/NGO,Foundation/Philanthropist,Government/Public Sector/Public Bank,Multilateral/Bilateral/Intergovernmental Financial Institution,Corporate Giving,Investment Fund,Other,"</formula1>
+      <formula1>"Nonprofit/NGO,Foundation/Philanthropist,Government/Public Sector/Public Bank,Multilateral/Bilateral/Intergovernmental Financial Institution,Corporate Giving,Investment Fund,Other"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F4:F32" type="list">
-      <formula1>"Interim,Overall,"</formula1>
+      <formula1>"Interim,Overall"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -7732,15 +7737,15 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L5:L33" type="list">
-      <formula1>"IRR,Average annual return,"</formula1>
+      <formula1>"IRR,Average annual return"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N5:N33" type="list">
-      <formula1>"No repayment (no principle or return),Some repayment (but below value of principle),Principal repaid (but no net return),Principal + positive financial returns,Not publicly available,"</formula1>
+      <formula1>"No repayment (no principle or return),Some repayment (but below value of principle),Principal repaid (but no net return),Principal + positive financial returns,Not publicly available"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O5:O33" type="list">
-      <formula1>"Debt,Equity,Combination,"</formula1>
+      <formula1>"Debt,Equity,Combination"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -8063,7 +8068,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B4:B32" type="list">
-      <formula1>"Impact bond design,Financial and commercial modeling,Impact bond investment structure,Capital raise ,Loan arranger,Performance management,Legal counsel,Technical assistance,Other,"</formula1>
+      <formula1>"Impact bond design,Financial and commercial modeling,Impact bond investment structure,Capital raise ,Loan arranger,Performance management,Legal counsel,Technical assistance,Other"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>